<commit_message>
Enhance dataset loading and configuration management; add multiprocessing and openpyxl dependencies. Update Jupyter notebooks for improved dataset handling and visualization. Refactor dashboard settings and utility functions for better clarity and functionality.
</commit_message>
<xml_diff>
--- a/crowd_certain/outputs/weight_strength_relation/ionosphere/weight_strength_relation.xlsx
+++ b/crowd_certain/outputs/weight_strength_relation/ionosphere/weight_strength_relation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>labelers_strength</t>
+          <t>workers_strength</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -449,21 +449,6 @@
           <t>accuracy-test</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>proposed</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>proposed_penalized</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Tao</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -473,396 +458,106 @@
         <v>0.2142857142857143</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4428571428571428</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.046027923707838</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.1233757615820099</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.000231069851095</v>
+        <v>0.4571428571428571</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>0.4164325559187557</v>
+        <v>0.4554031568612787</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4142857142857143</v>
+        <v>0.5285714285714286</v>
       </c>
       <c r="C3" t="n">
         <v>0.3285714285714286</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.8983322757138876</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.3083910085233472</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.000222091225445</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>0.4554031568612787</v>
+        <v>0.4880535344902678</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4571428571428571</v>
+        <v>0.4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3285714285714286</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.7897640249279304</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.5145163247637712</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.9983310227637663</v>
+        <v>0.5428571428571428</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>0.4842321631571403</v>
+        <v>0.5117561268266025</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3142857142857143</v>
+        <v>0.6142857142857143</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4428571428571428</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8642774832517891</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.5990754891476175</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.000227516810914</v>
+        <v>0.4142857142857143</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>0.4880535344902678</v>
+        <v>0.5813995435791038</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.791702277255097</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5751061458846574</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.000096778076017</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>0.5117561268266025</v>
+        <v>0.6073364362258287</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6714285714285714</v>
+        <v>0.7428571428571429</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4428571428571428</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8722142444660259</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.7722187200968778</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.9988889965663201</v>
+        <v>0.4571428571428571</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>0.5188608934509273</v>
+        <v>0.638060484538402</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5285714285714286</v>
+        <v>0.7428571428571429</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.786954441220026</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.6770912734483339</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.000175878112183</v>
+        <v>0.6285714285714286</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>0.5226713498389105</v>
+        <v>0.6502132028215444</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4</v>
+        <v>0.7428571428571429</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4714285714285714</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.9526730699998526</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.37329133103677</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.000227516538854</v>
+        <v>0.6285714285714286</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0.5813995435791038</v>
+        <v>0.7232900404020142</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7571428571428571</v>
+        <v>0.8142857142857143</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.872792138654563</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.97480380772015</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.00023159079406</v>
+        <v>0.7428571428571429</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>0.6073364362258287</v>
+        <v>0.8321946960652948</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8</v>
+        <v>0.8857142857142857</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4714285714285714</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.9260647473915009</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1.006211098419627</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.000154171139259</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>0.638060484538402</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1.046099301722793</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1.219885515398218</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1.000227998997609</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>0.6502132028215444</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.8142857142857143</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.6571428571428571</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1.020010057784988</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.215459087446978</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.00023339451694</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>0.6503828814202762</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.015181280714968</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1.243960114038624</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1.000232861127403</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>0.6515167086419769</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.7428571428571429</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.9215951205203533</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1.003168265118274</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.999118837887508</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>0.7232900404020142</v>
-      </c>
-      <c r="B16" t="n">
         <v>0.8428571428571429</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.6857142857142857</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1.195218123354168</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1.557058387910236</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1.000233393761815</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>0.735213897067451</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1.036657205276142</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1.30801534752387</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1.000233393761147</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>0.8022805061070414</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.222675948183255</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1.635309916323185</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1.000233334864703</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>0.8111317002380557</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.8285714285714286</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.7428571428571429</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.187449045544229</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1.5274638192273</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1.000233393408017</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>0.8321946960652948</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.9142857142857143</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.8714285714285714</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1.241059252954607</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1.638246709177389</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1.000233371955318</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>0.9268704618345672</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.313252037355989</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1.727351877212762</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1.000233387841628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>